<commit_message>
some changes on all agents and ACOPF fix
</commit_message>
<xml_diff>
--- a/applications/TransactiveEnergy/CoordinatorAgent/coordinator/finalsolution1.xlsx
+++ b/applications/TransactiveEnergy/CoordinatorAgent/coordinator/finalsolution1.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
   <si>
     <t>Bus ID</t>
   </si>
@@ -80,10 +80,160 @@
     <t>2006-01-01 00:05:00</t>
   </si>
   <si>
+    <t>0.997237265241</t>
+  </si>
+  <si>
+    <t>0.995982711648</t>
+  </si>
+  <si>
+    <t>0.994163593122</t>
+  </si>
+  <si>
+    <t>1.00000000007</t>
+  </si>
+  <si>
+    <t>0.995407611207</t>
+  </si>
+  <si>
+    <t>0.994659237504</t>
+  </si>
+  <si>
+    <t>0.995492318865</t>
+  </si>
+  <si>
+    <t>0.00502964971904</t>
+  </si>
+  <si>
+    <t>0.0240539493314</t>
+  </si>
+  <si>
+    <t>0.0446390551956</t>
+  </si>
+  <si>
+    <t>630.917934499</t>
+  </si>
+  <si>
+    <t>0.00114497922673</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>0.223008659203</t>
+  </si>
+  <si>
+    <t>0.0684772404772</t>
+  </si>
+  <si>
+    <t>0.111470118244</t>
+  </si>
+  <si>
+    <t>0.156409336706</t>
+  </si>
+  <si>
+    <t>0.997235429901</t>
+  </si>
+  <si>
+    <t>0.994161586927</t>
+  </si>
+  <si>
+    <t>7.09912129082e-11</t>
+  </si>
+  <si>
+    <t>0.00276273475934</t>
+  </si>
+  <si>
+    <t>0.00583640687768</t>
+  </si>
+  <si>
+    <t>-0.309772767994</t>
+  </si>
+  <si>
+    <t>-0.480589310068</t>
+  </si>
+  <si>
+    <t>-0.634052748596</t>
+  </si>
+  <si>
+    <t>-0.549622113727</t>
+  </si>
+  <si>
+    <t>-0.63747869098</t>
+  </si>
+  <si>
+    <t>-0.539686648751</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
     <t>2006-01-01 00:10:00</t>
+  </si>
+  <si>
+    <t>0.995982676901</t>
+  </si>
+  <si>
+    <t>0.995407261249</t>
+  </si>
+  <si>
+    <t>0.99465919259</t>
+  </si>
+  <si>
+    <t>0.995492139245</t>
+  </si>
+  <si>
+    <t>0.00471172697028</t>
+  </si>
+  <si>
+    <t>0.02443084203</t>
+  </si>
+  <si>
+    <t>0.0448455921824</t>
+  </si>
+  <si>
+    <t>630.917934436</t>
+  </si>
+  <si>
+    <t>0.00114491118914</t>
+  </si>
+  <si>
+    <t>0.000210970689415</t>
+  </si>
+  <si>
+    <t>0.221814870577</t>
+  </si>
+  <si>
+    <t>7.00857150093e-11</t>
+  </si>
+  <si>
+    <t>0.0027645700989</t>
+  </si>
+  <si>
+    <t>0.00583841307323</t>
+  </si>
+  <si>
+    <t>-0.309723721588</t>
+  </si>
+  <si>
+    <t>-0.48059199157</t>
+  </si>
+  <si>
+    <t>-0.634000652712</t>
+  </si>
+  <si>
+    <t>-0.549616410914</t>
+  </si>
+  <si>
+    <t>-0.637481758947</t>
+  </si>
+  <si>
+    <t>-0.539685918062</t>
   </si>
   <si>
     <t>2006-01-01 00:15:00</t>
@@ -467,74 +617,74 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -580,23 +730,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -654,41 +804,41 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -734,23 +884,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -817,65 +967,47 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -921,23 +1053,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -983,23 +1115,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1029,9 +1161,6 @@
       <c r="C1" t="n">
         <v>18</v>
       </c>
-      <c r="D1" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -1043,9 +1172,6 @@
       <c r="C2" t="n">
         <v>2</v>
       </c>
-      <c r="D2" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1057,41 +1183,32 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1121,9 +1238,6 @@
       <c r="C1" t="n">
         <v>18</v>
       </c>
-      <c r="D1" t="n">
-        <v>57</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -1135,9 +1249,6 @@
       <c r="C2" t="n">
         <v>2</v>
       </c>
-      <c r="D2" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1149,41 +1260,32 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1225,12 +1327,12 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1285,77 +1387,77 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1401,23 +1503,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1463,32 +1565,32 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1528,23 +1630,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1584,23 +1686,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1640,23 +1742,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1696,23 +1798,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1752,23 +1854,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1808,23 +1910,23 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some changes in ACOPF and others
</commit_message>
<xml_diff>
--- a/applications/TransactiveEnergy/CoordinatorAgent/coordinator/finalsolution1.xlsx
+++ b/applications/TransactiveEnergy/CoordinatorAgent/coordinator/finalsolution1.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>Bus ID</t>
   </si>
@@ -80,40 +80,40 @@
     <t>2006-01-01 00:05:00</t>
   </si>
   <si>
-    <t>0.997237265241</t>
-  </si>
-  <si>
-    <t>0.995982711648</t>
-  </si>
-  <si>
-    <t>0.994163593122</t>
-  </si>
-  <si>
-    <t>1.00000000007</t>
-  </si>
-  <si>
-    <t>0.995407611207</t>
-  </si>
-  <si>
-    <t>0.994659237504</t>
-  </si>
-  <si>
-    <t>0.995492318865</t>
-  </si>
-  <si>
-    <t>0.00502964971904</t>
-  </si>
-  <si>
-    <t>0.0240539493314</t>
-  </si>
-  <si>
-    <t>0.0446390551956</t>
-  </si>
-  <si>
-    <t>630.917934499</t>
-  </si>
-  <si>
-    <t>0.00114497922673</t>
+    <t>0.99726704192</t>
+  </si>
+  <si>
+    <t>0.996371849827</t>
+  </si>
+  <si>
+    <t>0.994981797879</t>
+  </si>
+  <si>
+    <t>0.999999999993</t>
+  </si>
+  <si>
+    <t>0.995760868528</t>
+  </si>
+  <si>
+    <t>0.994972502988</t>
+  </si>
+  <si>
+    <t>0.995845234483</t>
+  </si>
+  <si>
+    <t>0.00942434291958</t>
+  </si>
+  <si>
+    <t>0.0285816696422</t>
+  </si>
+  <si>
+    <t>0.05078081063</t>
+  </si>
+  <si>
+    <t>22.9136047221</t>
+  </si>
+  <si>
+    <t>0.00095193647401</t>
   </si>
   <si>
     <t>0.0</t>
@@ -125,49 +125,49 @@
     <t>2.0</t>
   </si>
   <si>
-    <t>0.223008659203</t>
-  </si>
-  <si>
-    <t>0.0684772404772</t>
-  </si>
-  <si>
-    <t>0.111470118244</t>
-  </si>
-  <si>
-    <t>0.156409336706</t>
-  </si>
-  <si>
-    <t>0.997235429901</t>
-  </si>
-  <si>
-    <t>0.994161586927</t>
-  </si>
-  <si>
-    <t>7.09912129082e-11</t>
-  </si>
-  <si>
-    <t>0.00276273475934</t>
-  </si>
-  <si>
-    <t>0.00583640687768</t>
-  </si>
-  <si>
-    <t>-0.309772767994</t>
-  </si>
-  <si>
-    <t>-0.480589310068</t>
-  </si>
-  <si>
-    <t>-0.634052748596</t>
-  </si>
-  <si>
-    <t>-0.549622113727</t>
-  </si>
-  <si>
-    <t>-0.63747869098</t>
-  </si>
-  <si>
-    <t>-0.539686648751</t>
+    <t>0.206</t>
+  </si>
+  <si>
+    <t>0.0901759779688</t>
+  </si>
+  <si>
+    <t>0.0800444515554</t>
+  </si>
+  <si>
+    <t>0.16316797363</t>
+  </si>
+  <si>
+    <t>0.997267041492</t>
+  </si>
+  <si>
+    <t>0.99498179723</t>
+  </si>
+  <si>
+    <t>-7.24897919469e-12</t>
+  </si>
+  <si>
+    <t>0.00273295808033</t>
+  </si>
+  <si>
+    <t>0.00501820212084</t>
+  </si>
+  <si>
+    <t>-0.292071520281</t>
+  </si>
+  <si>
+    <t>-0.433011165975</t>
+  </si>
+  <si>
+    <t>-0.535882795542</t>
+  </si>
+  <si>
+    <t>-0.506390440173</t>
+  </si>
+  <si>
+    <t>-0.5988777826</t>
+  </si>
+  <si>
+    <t>-0.496453177918</t>
   </si>
   <si>
     <t>0</t>
@@ -176,64 +176,61 @@
     <t>2006-01-01 00:10:00</t>
   </si>
   <si>
-    <t>0.995982676901</t>
-  </si>
-  <si>
-    <t>0.995407261249</t>
-  </si>
-  <si>
-    <t>0.99465919259</t>
-  </si>
-  <si>
-    <t>0.995492139245</t>
-  </si>
-  <si>
-    <t>0.00471172697028</t>
-  </si>
-  <si>
-    <t>0.02443084203</t>
-  </si>
-  <si>
-    <t>0.0448455921824</t>
-  </si>
-  <si>
-    <t>630.917934436</t>
-  </si>
-  <si>
-    <t>0.00114491118914</t>
-  </si>
-  <si>
-    <t>0.000210970689415</t>
-  </si>
-  <si>
-    <t>0.221814870577</t>
-  </si>
-  <si>
-    <t>7.00857150093e-11</t>
-  </si>
-  <si>
-    <t>0.0027645700989</t>
-  </si>
-  <si>
-    <t>0.00583841307323</t>
-  </si>
-  <si>
-    <t>-0.309723721588</t>
-  </si>
-  <si>
-    <t>-0.48059199157</t>
-  </si>
-  <si>
-    <t>-0.634000652712</t>
-  </si>
-  <si>
-    <t>-0.549616410914</t>
-  </si>
-  <si>
-    <t>-0.637481758947</t>
-  </si>
-  <si>
-    <t>-0.539685918062</t>
+    <t>0.996371849803</t>
+  </si>
+  <si>
+    <t>0.999999999984</t>
+  </si>
+  <si>
+    <t>0.995760868367</t>
+  </si>
+  <si>
+    <t>0.994972502961</t>
+  </si>
+  <si>
+    <t>0.99584523457</t>
+  </si>
+  <si>
+    <t>0.0093774913336</t>
+  </si>
+  <si>
+    <t>0.0286087428393</t>
+  </si>
+  <si>
+    <t>0.0507987123546</t>
+  </si>
+  <si>
+    <t>22.9136047224</t>
+  </si>
+  <si>
+    <t>0.000951936411409</t>
+  </si>
+  <si>
+    <t>-1.64188662666e-11</t>
+  </si>
+  <si>
+    <t>0.00273295850764</t>
+  </si>
+  <si>
+    <t>0.00501820276989</t>
+  </si>
+  <si>
+    <t>-0.292071508719</t>
+  </si>
+  <si>
+    <t>-0.433011165847</t>
+  </si>
+  <si>
+    <t>-0.535882777898</t>
+  </si>
+  <si>
+    <t>-0.506390436147</t>
+  </si>
+  <si>
+    <t>-0.598877782288</t>
+  </si>
+  <si>
+    <t>-0.496453180854</t>
   </si>
   <si>
     <t>2006-01-01 00:15:00</t>
@@ -649,21 +646,21 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>34</v>
@@ -675,16 +672,16 @@
         <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -738,15 +735,15 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -829,7 +826,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>31</v>
@@ -892,15 +889,15 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -987,10 +984,10 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -999,15 +996,15 @@
         <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1061,15 +1058,15 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1123,15 +1120,15 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1194,21 +1191,21 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
         <v>59</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1271,21 +1268,21 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
         <v>59</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1332,7 +1329,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1413,22 +1410,22 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>62</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>63</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>64</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>65</v>
-      </c>
-      <c r="G5" t="s">
-        <v>66</v>
       </c>
       <c r="H5" t="s">
         <v>45</v>
@@ -1436,25 +1433,25 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>62</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>64</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>65</v>
-      </c>
-      <c r="G6" t="s">
-        <v>66</v>
       </c>
       <c r="H6" t="s">
         <v>45</v>
@@ -1511,15 +1508,15 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1576,21 +1573,21 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1638,15 +1635,15 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1694,15 +1691,15 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1755,7 +1752,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -1806,15 +1803,15 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1867,7 +1864,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
@@ -1923,7 +1920,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>

</xml_diff>